<commit_message>
Move Gridlines from Chart to Axis
This could, I hope, be my last major change to Chart for a while. When I first noticed this problem, I thought it would be a breaking change. However, although this change establishes some deprecations, I don't think it breaks anything. Major and minor gridlines had only been settable by the Chart constructor. This PR moves them where they belong, to Axis (eexisting Chart constructor code will still work). This allows them to be specified from both X and Y axis.

Chart is now entirely covered except for 2 statements, one deprecated and one that I just can't figure out. 99.71% for Charts, 88.96% overall. All references to the Chart directory in Phpstan baseline are eliminated.
</commit_message>
<xml_diff>
--- a/samples/templates/32readwriteLineChart4.xlsx
+++ b/samples/templates/32readwriteLineChart4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\chartgrid\samples\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A30CA73-B927-42E7-9811-6F86AF4EB46E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAC3D37-E981-4420-97B7-C3B2AD5EAE3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -436,6 +436,16 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -885,7 +895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>